<commit_message>
MT Stock Report & GT Permanent Stock
</commit_message>
<xml_diff>
--- a/assets/templates/MT_Stock_Tracker.xlsx
+++ b/assets/templates/MT_Stock_Tracker.xlsx
@@ -15,7 +15,7 @@
     <sheet name="STORE FILE" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STORE FILE'!$A$8:$T$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'STORE FILE'!$A$8:$U$119</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>PAPAYA</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +417,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,22 +435,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -730,7 +719,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:BY100"/>
+  <dimension ref="A1:BZ100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -748,29 +737,29 @@
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="39" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="44" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="9.140625" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" customWidth="1"/>
-    <col min="47" max="47" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="55" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="60" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="8.85546875" collapsed="1"/>
-    <col min="63" max="63" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="71" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="72" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="76" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="77" max="77" width="9.140625" collapsed="1"/>
-    <col min="78" max="78" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="40" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="45" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="9.140625" collapsed="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
+    <col min="48" max="48" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="56" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="61" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="8.85546875" collapsed="1"/>
+    <col min="64" max="64" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="72" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="73" max="73" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="74" max="77" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="78" max="78" width="9.140625" collapsed="1"/>
+    <col min="79" max="79" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -778,7 +767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
@@ -791,13 +780,13 @@
       <c r="F2" s="2">
         <v>20</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
@@ -821,7 +810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
@@ -842,11 +831,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -855,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:76" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="K7" s="11" t="s">
@@ -864,57 +853,58 @@
       <c r="L7" s="12">
         <v>43467</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="M7" s="16"/>
+      <c r="V7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16" t="s">
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AC7" s="12" t="s">
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AD7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AM7" s="16" t="s">
+      <c r="AN7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AN7" s="16"/>
-      <c r="AO7" s="16"/>
-      <c r="AP7" s="16" t="s">
+      <c r="AO7" s="17"/>
+      <c r="AP7" s="17"/>
+      <c r="AQ7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="AQ7" s="16"/>
-      <c r="AR7" s="16"/>
-      <c r="AT7" s="12" t="s">
+      <c r="AR7" s="17"/>
+      <c r="AS7" s="17"/>
+      <c r="AU7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="BC7" s="16" t="s">
+      <c r="BD7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="BD7" s="16"/>
-      <c r="BE7" s="16"/>
-      <c r="BF7" s="16" t="s">
+      <c r="BE7" s="17"/>
+      <c r="BF7" s="17"/>
+      <c r="BG7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="BG7" s="16"/>
-      <c r="BH7" s="16"/>
-      <c r="BJ7" s="12" t="s">
+      <c r="BH7" s="17"/>
+      <c r="BI7" s="17"/>
+      <c r="BK7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="BS7" s="16" t="s">
+      <c r="BT7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="BT7" s="16"/>
-      <c r="BU7" s="16"/>
-      <c r="BV7" s="16" t="s">
+      <c r="BU7" s="17"/>
+      <c r="BV7" s="17"/>
+      <c r="BW7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="BW7" s="16"/>
-      <c r="BX7" s="16"/>
+      <c r="BX7" s="17"/>
+      <c r="BY7" s="17"/>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -947,190 +937,193 @@
         <v>29</v>
       </c>
       <c r="L8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="P8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="13" t="s">
+      <c r="Q8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="13" t="s">
+      <c r="R8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="13" t="s">
+      <c r="S8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="U8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="V8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="V8" s="13" t="s">
+      <c r="W8" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="W8" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="Y8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Z8" s="13" t="s">
+      <c r="AA8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AA8" s="15"/>
       <c r="AB8" s="15"/>
-      <c r="AC8" s="13" t="s">
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AD8" s="13" t="s">
+      <c r="AE8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AE8" s="13" t="s">
+      <c r="AF8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AF8" s="13" t="s">
+      <c r="AG8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AG8" s="13" t="s">
+      <c r="AH8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AH8" s="13" t="s">
+      <c r="AI8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AI8" s="13" t="s">
+      <c r="AJ8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AJ8" s="13" t="s">
+      <c r="AK8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AK8" s="13" t="s">
+      <c r="AL8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AL8" s="13" t="s">
+      <c r="AM8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AM8" s="13" t="s">
+      <c r="AN8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AN8" s="13" t="s">
+      <c r="AO8" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="AO8" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="AP8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="AQ8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AR8" s="13" t="s">
+      <c r="AS8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AS8" s="15"/>
-      <c r="AT8" s="13" t="s">
+      <c r="AT8" s="15"/>
+      <c r="AU8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AU8" s="13" t="s">
+      <c r="AV8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AV8" s="13" t="s">
+      <c r="AW8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AW8" s="13" t="s">
+      <c r="AX8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="AX8" s="13" t="s">
+      <c r="AY8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="AY8" s="13" t="s">
+      <c r="AZ8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AZ8" s="13" t="s">
+      <c r="BA8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="BA8" s="13" t="s">
+      <c r="BB8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="BB8" s="13" t="s">
+      <c r="BC8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="BC8" s="13" t="s">
+      <c r="BD8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="BD8" s="13" t="s">
+      <c r="BE8" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="BE8" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="BF8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="BG8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="BH8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="BH8" s="13" t="s">
+      <c r="BI8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="BI8" s="15"/>
-      <c r="BJ8" s="13" t="s">
+      <c r="BJ8" s="15"/>
+      <c r="BK8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="BK8" s="13" t="s">
+      <c r="BL8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="BL8" s="13" t="s">
+      <c r="BM8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="BM8" s="13" t="s">
+      <c r="BN8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="BN8" s="13" t="s">
+      <c r="BO8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="BO8" s="13" t="s">
+      <c r="BP8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="BP8" s="13" t="s">
+      <c r="BQ8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="BQ8" s="13" t="s">
+      <c r="BR8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="BR8" s="13" t="s">
+      <c r="BS8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="BS8" s="13" t="s">
+      <c r="BT8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="BT8" s="13" t="s">
+      <c r="BU8" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="BU8" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="BV8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="BW8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="BX8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="BX8" s="13" t="s">
+      <c r="BY8" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1215,15 +1208,15 @@
     <sortCondition ref="B18:B116"/>
   </sortState>
   <mergeCells count="9">
-    <mergeCell ref="BC7:BE7"/>
-    <mergeCell ref="BF7:BH7"/>
-    <mergeCell ref="BS7:BU7"/>
-    <mergeCell ref="BV7:BX7"/>
+    <mergeCell ref="BD7:BF7"/>
+    <mergeCell ref="BG7:BI7"/>
+    <mergeCell ref="BT7:BV7"/>
+    <mergeCell ref="BW7:BY7"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AM7:AO7"/>
-    <mergeCell ref="AP7:AR7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AN7:AP7"/>
+    <mergeCell ref="AQ7:AS7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>